<commit_message>
feat(core): apply global row rules to Schema Editor and update test data
- Fix Schema Editor to ignore 1st row and use 2nd row as header

- Filter out headers starting with '#' in Schema Editor

- Update external test Excel files to match global row rules (1st row dummy)
</commit_message>
<xml_diff>
--- a/ExternalTestData/Excel/FilterTest.xlsx
+++ b/ExternalTestData/Excel/FilterTest.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -58,6 +58,9 @@
   <si>
     <t xml:space="preserve">3000</t>
   </si>
+  <si>
+    <t xml:space="preserve"># Dummy Row (Ignored by ExcelBinder)</t>
+  </si>
 </sst>
 </file>
 
@@ -101,7 +104,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="1" showOutlineSymbols="1" defaultGridColor="1" colorId="64" zoomScale="100" workbookViewId="0"/>
   </sheetViews>
@@ -109,57 +112,62 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B5" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C5" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D5" s="0" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>